<commit_message>
Updating dates for Forecasting
</commit_message>
<xml_diff>
--- a/Monthly_Cost_For_JUN_2025.xlsx
+++ b/Monthly_Cost_For_JUN_2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G183"/>
+  <dimension ref="A1:G184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.0157149948</v>
+        <v>0.0288336093</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1.0810040434</v>
+        <v>1.8552575123</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>103.9196388204</v>
+        <v>174.0418963931</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.34</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -668,7 +668,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>AWS CloudFormation</t>
+          <t>AWS Certificate Manager</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -676,7 +676,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -703,11 +703,11 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>AWS CloudTrail</t>
+          <t>AWS CloudFormation</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>1936.8965197583</v>
+        <v>0</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -738,11 +738,11 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>AWS Config</t>
+          <t>AWS CloudTrail</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>1272.928</v>
+        <v>3235.0527912963</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -773,11 +773,11 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>AWS Cost Explorer</t>
+          <t>AWS Config</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>67.76000000000001</v>
+        <v>2046.294</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -808,11 +808,11 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>AWS DataSync</t>
+          <t>AWS Cost Explorer</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>7.8913207809</v>
+        <v>115.83</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -847,11 +847,11 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>17.657183881</v>
+        <v>12.7589974605</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -878,15 +878,15 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>AWS Database Migration Service</t>
+          <t>AWS DataSync</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>1718.5998333578</v>
+        <v>85.4769308141</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -917,11 +917,11 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>167.2582110948</v>
+        <v>2273.8211666986</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -948,15 +948,15 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>AWS Direct Connect</t>
+          <t>AWS Database Migration Service</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>578.3631294504</v>
+        <v>275.725388862</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -983,11 +983,11 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>AWS Directory Service</t>
+          <t>AWS Direct Connect</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>267.446996139</v>
+        <v>1030.9076819671</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1018,11 +1018,11 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>AWS Elemental MediaLive</t>
+          <t>AWS Directory Service</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>14.68</v>
+        <v>440.9516286361</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1053,11 +1053,11 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>AWS Elemental MediaStore</t>
+          <t>AWS Elemental MediaLive</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>9.70424e-05</v>
+        <v>24.2</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1088,11 +1088,11 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>AWS End User Messaging</t>
+          <t>AWS Elemental MediaStore</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1.5291666789</v>
+        <v>0.0001607598</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1123,15 +1123,15 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>AWS Global Accelerator</t>
+          <t>AWS End User Messaging</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>18.35</v>
+        <v>2.5208333535</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -1158,15 +1158,15 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>AWS Glue</t>
+          <t>AWS Global Accelerator</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>1.88156364</v>
+        <v>30.25</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -1193,11 +1193,11 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>AWS Key Management Service</t>
+          <t>AWS Glue</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>86.76534132419999</v>
+        <v>3.17580076</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1232,11 +1232,11 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>1.2631526766</v>
+        <v>144.6108845413</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -1267,11 +1267,11 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>0.5044217818</v>
+        <v>1.9278491263</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -1302,11 +1302,11 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>0.5105892263</v>
+        <v>0.8357214511</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Environment$loadtest</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -1337,11 +1337,11 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>34.9896772594</v>
+        <v>0.8416937845</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$loadtest</t>
         </is>
       </c>
     </row>
@@ -1372,11 +1372,11 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>32.5126992715</v>
+        <v>58.2617874677</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -1407,11 +1407,11 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>1.0111111192</v>
+        <v>53.8145072655</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Environment$shared</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -1442,11 +1442,11 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>0.5032697818</v>
+        <v>1.6708333467</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$shared</t>
         </is>
       </c>
     </row>
@@ -1473,15 +1473,15 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>AWS Lambda</t>
+          <t>AWS Key Management Service</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>974.8213515872</v>
+        <v>0.8327634511000001</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -1512,11 +1512,11 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>5.0682413908</v>
+        <v>1468.2236937813</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Environment$Development</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -1547,11 +1547,11 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>23.1066445647</v>
+        <v>8.2761562333</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$Development</t>
         </is>
       </c>
     </row>
@@ -1582,11 +1582,11 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>0.4489631975</v>
+        <v>41.1988676852</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -1617,11 +1617,11 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>0.5628492099</v>
+        <v>0.7468858869</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -1652,11 +1652,11 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>3.0440715189</v>
+        <v>0.9372952451</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -1687,11 +1687,11 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>7.3271536003</v>
+        <v>5.0647716668</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -1722,11 +1722,11 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>0.3838458329</v>
+        <v>12.2319838307</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -1753,15 +1753,15 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>AWS Secrets Manager</t>
+          <t>AWS Lambda</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>50.5490378754</v>
+        <v>0.6380465423</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -1792,11 +1792,11 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>0.1795307395</v>
+        <v>82.821738213</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -1827,11 +1827,11 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>35.6954735717</v>
+        <v>0.3939329723</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -1862,11 +1862,11 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>41.5252352373</v>
+        <v>58.6708052117</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -1893,15 +1893,15 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>AWS Security Hub</t>
+          <t>AWS Secrets Manager</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>128.11418</v>
+        <v>68.5413240149</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -1928,11 +1928,11 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>AWS Step Functions</t>
+          <t>AWS Security Hub</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>0.00063126</v>
+        <v>192.15931</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -1963,11 +1963,11 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>AWS Support (Business)</t>
+          <t>AWS Step Functions</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>213.3436100019</v>
+        <v>0.0009195857999999999</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -1998,11 +1998,11 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>AWS Support (Enterprise)</t>
+          <t>AWS Support (Business)</t>
         </is>
       </c>
       <c r="F45" t="n">
-        <v>27037.83</v>
+        <v>349.8301485498</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -2033,11 +2033,11 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>AWS Systems Manager</t>
+          <t>AWS Support (Enterprise)</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>0.07707</v>
+        <v>39275.23</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -2068,11 +2068,11 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>AWS Transfer Family</t>
+          <t>AWS Systems Manager</t>
         </is>
       </c>
       <c r="F47" t="n">
-        <v>110.4201875418</v>
+        <v>0.12705</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -2103,11 +2103,11 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>AWS WAF</t>
+          <t>AWS Transfer Family</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>55.2735730514</v>
+        <v>182.0056969914</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -2142,11 +2142,11 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>5.7500186526</v>
+        <v>91.0312301254</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2177,11 +2177,11 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>712.8767570526001</v>
+        <v>9.539895369</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2208,15 +2208,15 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>AWS X-Ray</t>
+          <t>AWS WAF</t>
         </is>
       </c>
       <c r="F51" t="n">
-        <v>25.5935675</v>
+        <v>1199.423308569</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -2243,11 +2243,11 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Amazon API Gateway</t>
+          <t>AWS X-Ray</t>
         </is>
       </c>
       <c r="F52" t="n">
-        <v>144.434148831</v>
+        <v>43.102505</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2278,11 +2278,11 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Amazon Athena</t>
+          <t>Amazon API Gateway</t>
         </is>
       </c>
       <c r="F53" t="n">
-        <v>63.9016</v>
+        <v>236.7473786515</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2313,11 +2313,11 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Amazon CloudFront</t>
+          <t>Amazon Athena</t>
         </is>
       </c>
       <c r="F54" t="n">
-        <v>7356.165797624</v>
+        <v>75.844995</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2352,11 +2352,11 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>0.097314636</v>
+        <v>12429.8175006762</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2387,11 +2387,11 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>1.0816768045</v>
+        <v>0.1829593319</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2422,11 +2422,11 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>2805.8561113364</v>
+        <v>1.8283606754</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -2457,11 +2457,11 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>0.0291297722</v>
+        <v>4690.6364164779</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Environment$qa</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -2492,11 +2492,11 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>5.339e-07</v>
+        <v>0.0587891736</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$qa</t>
         </is>
       </c>
     </row>
@@ -2523,15 +2523,15 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Amazon Cognito</t>
+          <t>Amazon CloudFront</t>
         </is>
       </c>
       <c r="F60" t="n">
-        <v>163.8675</v>
+        <v>8.583e-07</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -2558,11 +2558,11 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Amazon Detective</t>
+          <t>Amazon Cognito</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>59.4930339384</v>
+        <v>173.184</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -2593,11 +2593,11 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Amazon DevOps Guru</t>
+          <t>Amazon Detective</t>
         </is>
       </c>
       <c r="F62" t="n">
-        <v>0</v>
+        <v>99.969167674</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2628,11 +2628,11 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Amazon DocumentDB (with MongoDB compatibility)</t>
+          <t>Amazon DevOps Guru</t>
         </is>
       </c>
       <c r="F63" t="n">
-        <v>0.0812354663</v>
+        <v>0</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2667,11 +2667,11 @@
         </is>
       </c>
       <c r="F64" t="n">
-        <v>135.8431970614</v>
+        <v>0.1332322401</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2702,11 +2702,11 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>105.7014521814</v>
+        <v>224.1591953311</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2733,15 +2733,15 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Amazon DynamoDB</t>
+          <t>Amazon DocumentDB (with MongoDB compatibility)</t>
         </is>
       </c>
       <c r="F66" t="n">
-        <v>26.3810214165</v>
+        <v>174.4443996095</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -2772,11 +2772,11 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>25.904008987</v>
+        <v>59.2951093628</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2807,11 +2807,11 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>67.4319984041</v>
+        <v>44.1365828603</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2838,15 +2838,15 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Amazon EC2 Container Registry (ECR)</t>
+          <t>Amazon DynamoDB</t>
         </is>
       </c>
       <c r="F69" t="n">
-        <v>67.53453917820001</v>
+        <v>108.7927429152</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -2877,11 +2877,11 @@
         </is>
       </c>
       <c r="F70" t="n">
-        <v>0.0186602618</v>
+        <v>111.2735852756</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Environment$common</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2912,11 +2912,11 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>0.204918854</v>
+        <v>0.030761467</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$common</t>
         </is>
       </c>
     </row>
@@ -2947,11 +2947,11 @@
         </is>
       </c>
       <c r="F72" t="n">
-        <v>452.1623601133</v>
+        <v>0.3378085658</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2978,15 +2978,15 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Amazon ElastiCache</t>
+          <t>Amazon EC2 Container Registry (ECR)</t>
         </is>
       </c>
       <c r="F73" t="n">
-        <v>7309.0435649224</v>
+        <v>746.3039955038</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3017,11 +3017,11 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>3364.9566983325</v>
+        <v>9873.9905066224</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3052,11 +3052,11 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>2876.6928</v>
+        <v>5546.4426983325</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3083,15 +3083,15 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>EC2 - Other</t>
+          <t>Amazon ElastiCache</t>
         </is>
       </c>
       <c r="F76" t="n">
-        <v>12262.1375421669</v>
+        <v>4721.5584</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3122,11 +3122,11 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>0.3922222183</v>
+        <v>20433.5433826712</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Environment$PSFalcon</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3157,11 +3157,11 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>7.9415541049</v>
+        <v>0.6677777711</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$PSFalcon</t>
         </is>
       </c>
     </row>
@@ -3192,11 +3192,11 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>0.9063003983</v>
+        <v>7.9415541049</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -3227,11 +3227,11 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>9.8055555634</v>
+        <v>1.4760347671</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Environment$management</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -3262,11 +3262,11 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>690.2742489372</v>
+        <v>16.6944444578</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$management</t>
         </is>
       </c>
     </row>
@@ -3297,11 +3297,11 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>10.0500839453</v>
+        <v>1279.4651480673</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3332,11 +3332,11 @@
         </is>
       </c>
       <c r="F83" t="n">
-        <v>3466.9257995079</v>
+        <v>16.0616635355</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -3367,11 +3367,11 @@
         </is>
       </c>
       <c r="F84" t="n">
-        <v>0.4407615353</v>
+        <v>5808.3695991941</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3398,15 +3398,15 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Amazon Elastic Compute Cloud - Compute</t>
+          <t>EC2 - Other</t>
         </is>
       </c>
       <c r="F85" t="n">
-        <v>9077.3013732855</v>
+        <v>0.7109613648000001</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -3437,11 +3437,11 @@
         </is>
       </c>
       <c r="F86" t="n">
-        <v>0.106892501</v>
+        <v>14580.3008416892</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3472,11 +3472,11 @@
         </is>
       </c>
       <c r="F87" t="n">
-        <v>31.6224</v>
+        <v>0.106892501</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -3507,11 +3507,11 @@
         </is>
       </c>
       <c r="F88" t="n">
-        <v>3851.7807439905</v>
+        <v>52.0992</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -3542,11 +3542,11 @@
         </is>
       </c>
       <c r="F89" t="n">
-        <v>0</v>
+        <v>5851.3774811353</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3577,11 +3577,11 @@
         </is>
       </c>
       <c r="F90" t="n">
-        <v>33371.5026949729</v>
+        <v>0</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -3612,11 +3612,11 @@
         </is>
       </c>
       <c r="F91" t="n">
-        <v>0</v>
+        <v>55772.7317472135</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3643,15 +3643,15 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Amazon Elastic Container Service</t>
+          <t>Amazon Elastic Compute Cloud - Compute</t>
         </is>
       </c>
       <c r="F92" t="n">
-        <v>3962.2004624565</v>
+        <v>0</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -3678,11 +3678,11 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Amazon Elastic Container Service for Kubernetes</t>
+          <t>Amazon Elastic Container Service</t>
         </is>
       </c>
       <c r="F93" t="n">
-        <v>280.2216122315</v>
+        <v>6209.8097400529</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3717,11 +3717,11 @@
         </is>
       </c>
       <c r="F94" t="n">
-        <v>330.3</v>
+        <v>458.2914754534</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3752,11 +3752,11 @@
         </is>
       </c>
       <c r="F95" t="n">
-        <v>330.3</v>
+        <v>544.5</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3783,15 +3783,15 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Amazon Elastic File System</t>
+          <t>Amazon Elastic Container Service for Kubernetes</t>
         </is>
       </c>
       <c r="F96" t="n">
-        <v>40.1757997205</v>
+        <v>544.5</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3818,11 +3818,11 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Amazon Elastic Load Balancing</t>
+          <t>Amazon Elastic File System</t>
         </is>
       </c>
       <c r="F97" t="n">
-        <v>3651.4842257856</v>
+        <v>66.2296925137</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3857,11 +3857,11 @@
         </is>
       </c>
       <c r="F98" t="n">
-        <v>8.257596794399999</v>
+        <v>5913.5322371637</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3892,11 +3892,11 @@
         </is>
       </c>
       <c r="F99" t="n">
-        <v>8.306769154099999</v>
+        <v>13.6126682955</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -3927,11 +3927,11 @@
         </is>
       </c>
       <c r="F100" t="n">
-        <v>165.2684504568</v>
+        <v>13.6950270879</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -3962,11 +3962,11 @@
         </is>
       </c>
       <c r="F101" t="n">
-        <v>24.7757145543</v>
+        <v>274.8654757742</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3997,11 +3997,11 @@
         </is>
       </c>
       <c r="F102" t="n">
-        <v>1081.4975191026</v>
+        <v>35.1269179749</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -4032,11 +4032,11 @@
         </is>
       </c>
       <c r="F103" t="n">
-        <v>8.301672612200001</v>
+        <v>1800.0183642364</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -4063,15 +4063,15 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Amazon Elastic Transcoder</t>
+          <t>Amazon Elastic Load Balancing</t>
         </is>
       </c>
       <c r="F104" t="n">
-        <v>0.6345</v>
+        <v>13.6843288862</v>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -4098,11 +4098,11 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Amazon Glacier</t>
+          <t>Amazon Elastic Transcoder</t>
         </is>
       </c>
       <c r="F105" t="n">
-        <v>1.2903913597</v>
+        <v>0.7425</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
@@ -4133,11 +4133,11 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Amazon GuardDuty</t>
+          <t>Amazon Glacier</t>
         </is>
       </c>
       <c r="F106" t="n">
-        <v>1846.0666022583</v>
+        <v>2.1506528493</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
@@ -4168,11 +4168,11 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Amazon Inspector</t>
+          <t>Amazon GuardDuty</t>
         </is>
       </c>
       <c r="F107" t="n">
-        <v>1.2</v>
+        <v>2826.6792645572</v>
       </c>
       <c r="G107" t="inlineStr">
         <is>
@@ -4203,11 +4203,11 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Amazon Kinesis</t>
+          <t>Amazon Inspector</t>
         </is>
       </c>
       <c r="F108" t="n">
-        <v>55.05</v>
+        <v>1.8</v>
       </c>
       <c r="G108" t="inlineStr">
         <is>
@@ -4238,11 +4238,11 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Amazon Lightsail</t>
+          <t>Amazon Kinesis</t>
         </is>
       </c>
       <c r="F109" t="n">
-        <v>5.2432547396</v>
+        <v>90.75</v>
       </c>
       <c r="G109" t="inlineStr">
         <is>
@@ -4273,11 +4273,11 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Amazon Location Service</t>
+          <t>Amazon Lightsail</t>
         </is>
       </c>
       <c r="F110" t="n">
-        <v>0.0003985</v>
+        <v>8.6349089709</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
@@ -4308,11 +4308,11 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Amazon MQ</t>
+          <t>Amazon Location Service</t>
         </is>
       </c>
       <c r="F111" t="n">
-        <v>32.9867117562</v>
+        <v>0.000647</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
@@ -4347,11 +4347,11 @@
         </is>
       </c>
       <c r="F112" t="n">
-        <v>115.7880375358</v>
+        <v>54.3792610816</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4382,11 +4382,11 @@
         </is>
       </c>
       <c r="F113" t="n">
-        <v>115.8093147425</v>
+        <v>191.2108822634</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -4413,15 +4413,15 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Amazon Macie</t>
+          <t>Amazon MQ</t>
         </is>
       </c>
       <c r="F114" t="n">
-        <v>1.28232</v>
+        <v>191.2530218341</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -4448,11 +4448,11 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Amazon Managed Grafana</t>
+          <t>Amazon Macie</t>
         </is>
       </c>
       <c r="F115" t="n">
-        <v>9</v>
+        <v>2.1372</v>
       </c>
       <c r="G115" t="inlineStr">
         <is>
@@ -4483,11 +4483,11 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Amazon Managed Workflows for Apache Airflow</t>
+          <t>Amazon Managed Grafana</t>
         </is>
       </c>
       <c r="F116" t="n">
-        <v>1802.5781504698</v>
+        <v>9</v>
       </c>
       <c r="G116" t="inlineStr">
         <is>
@@ -4522,11 +4522,11 @@
         </is>
       </c>
       <c r="F117" t="n">
-        <v>631.5181753076</v>
+        <v>2844.0085244428</v>
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4557,11 +4557,11 @@
         </is>
       </c>
       <c r="F118" t="n">
-        <v>1816.3087898868</v>
+        <v>983.263232046</v>
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -4588,15 +4588,15 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Amazon Neptune</t>
+          <t>Amazon Managed Workflows for Apache Airflow</t>
         </is>
       </c>
       <c r="F119" t="n">
-        <v>2.4204078456</v>
+        <v>2993.4019758456</v>
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -4623,11 +4623,11 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Amazon OpenSearch Service</t>
+          <t>Amazon Neptune</t>
         </is>
       </c>
       <c r="F120" t="n">
-        <v>300.5947131244</v>
+        <v>4.0443665759</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
@@ -4662,11 +4662,11 @@
         </is>
       </c>
       <c r="F121" t="n">
-        <v>5101.4539012871</v>
+        <v>495.528989664</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4697,11 +4697,11 @@
         </is>
       </c>
       <c r="F122" t="n">
-        <v>15398.0706068171</v>
+        <v>8450.8530918409</v>
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -4728,15 +4728,15 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Amazon Personalize</t>
+          <t>Amazon OpenSearch Service</t>
         </is>
       </c>
       <c r="F123" t="n">
-        <v>293.597064</v>
+        <v>25383.7398945714</v>
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -4763,11 +4763,11 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Amazon QuickSight</t>
+          <t>Amazon Personalize</t>
         </is>
       </c>
       <c r="F124" t="n">
-        <v>32.6073596805</v>
+        <v>483.99516</v>
       </c>
       <c r="G124" t="inlineStr">
         <is>
@@ -4798,11 +4798,11 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Amazon Redshift</t>
+          <t>Amazon QuickSight</t>
         </is>
       </c>
       <c r="F125" t="n">
-        <v>207.17392945</v>
+        <v>53.7532768575</v>
       </c>
       <c r="G125" t="inlineStr">
         <is>
@@ -4833,11 +4833,11 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Amazon Relational Database Service</t>
+          <t>Amazon Redshift</t>
         </is>
       </c>
       <c r="F126" t="n">
-        <v>36158.3655218608</v>
+        <v>341.53970508</v>
       </c>
       <c r="G126" t="inlineStr">
         <is>
@@ -4872,11 +4872,11 @@
         </is>
       </c>
       <c r="F127" t="n">
-        <v>0.00086598</v>
+        <v>53712.4170909383</v>
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>Environment$loadtest</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4907,11 +4907,11 @@
         </is>
       </c>
       <c r="F128" t="n">
-        <v>1122.6722618464</v>
+        <v>0.0014408945</v>
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$loadtest</t>
         </is>
       </c>
     </row>
@@ -4942,11 +4942,11 @@
         </is>
       </c>
       <c r="F129" t="n">
-        <v>3542.3381397678</v>
+        <v>1748.8903300706</v>
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -4973,15 +4973,15 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Amazon Route 53</t>
+          <t>Amazon Relational Database Service</t>
         </is>
       </c>
       <c r="F130" t="n">
-        <v>1069.2117381051</v>
+        <v>6066.6779007892</v>
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -5012,11 +5012,11 @@
         </is>
       </c>
       <c r="F131" t="n">
-        <v>0.1721436</v>
+        <v>1548.9976323009</v>
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>Environment$Dev</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -5047,11 +5047,11 @@
         </is>
       </c>
       <c r="F132" t="n">
-        <v>0.1</v>
+        <v>0.2014698</v>
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$Dev</t>
         </is>
       </c>
     </row>
@@ -5086,7 +5086,7 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>Environment$common</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -5117,11 +5117,11 @@
         </is>
       </c>
       <c r="F134" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>Environment$global</t>
+          <t>Environment$common</t>
         </is>
       </c>
     </row>
@@ -5152,11 +5152,11 @@
         </is>
       </c>
       <c r="F135" t="n">
-        <v>0.100171</v>
+        <v>0.5</v>
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>Environment$loadtest</t>
+          <t>Environment$global</t>
         </is>
       </c>
     </row>
@@ -5187,11 +5187,11 @@
         </is>
       </c>
       <c r="F136" t="n">
-        <v>6.2350756</v>
+        <v>0.100243</v>
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$loadtest</t>
         </is>
       </c>
     </row>
@@ -5222,11 +5222,11 @@
         </is>
       </c>
       <c r="F137" t="n">
-        <v>8.2111918</v>
+        <v>6.9405616</v>
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -5257,11 +5257,11 @@
         </is>
       </c>
       <c r="F138" t="n">
-        <v>0.1001474</v>
+        <v>11.1678916</v>
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>Environment$sandbox</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -5292,11 +5292,11 @@
         </is>
       </c>
       <c r="F139" t="n">
-        <v>0.100015</v>
+        <v>0.1002096</v>
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$sandbox</t>
         </is>
       </c>
     </row>
@@ -5327,11 +5327,11 @@
         </is>
       </c>
       <c r="F140" t="n">
-        <v>0.1</v>
+        <v>0.1000202</v>
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>Environment$test</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -5358,15 +5358,15 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Amazon SageMaker</t>
+          <t>Amazon Route 53</t>
         </is>
       </c>
       <c r="F141" t="n">
-        <v>625.2528096983</v>
+        <v>0.1</v>
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$test</t>
         </is>
       </c>
     </row>
@@ -5393,11 +5393,11 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Amazon Simple Email Service</t>
+          <t>Amazon SageMaker</t>
         </is>
       </c>
       <c r="F142" t="n">
-        <v>8.2792289437</v>
+        <v>1031.1527075889</v>
       </c>
       <c r="G142" t="inlineStr">
         <is>
@@ -5428,11 +5428,11 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Amazon Simple Notification Service</t>
+          <t>Amazon Simple Email Service</t>
         </is>
       </c>
       <c r="F143" t="n">
-        <v>9.115520739700001</v>
+        <v>13.9081457955</v>
       </c>
       <c r="G143" t="inlineStr">
         <is>
@@ -5467,11 +5467,11 @@
         </is>
       </c>
       <c r="F144" t="n">
-        <v>0.0042219733</v>
+        <v>15.5977678793</v>
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>Environment$Common</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -5502,11 +5502,11 @@
         </is>
       </c>
       <c r="F145" t="n">
-        <v>0.0005455</v>
+        <v>0.0075156443</v>
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$Common</t>
         </is>
       </c>
     </row>
@@ -5537,11 +5537,11 @@
         </is>
       </c>
       <c r="F146" t="n">
-        <v>3.5e-06</v>
+        <v>0.000922</v>
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>Environment$Sandbox</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -5572,11 +5572,11 @@
         </is>
       </c>
       <c r="F147" t="n">
-        <v>0.0005465</v>
+        <v>6e-06</v>
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$Sandbox</t>
         </is>
       </c>
     </row>
@@ -5603,15 +5603,15 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>Amazon Simple Queue Service</t>
+          <t>Amazon Simple Notification Service</t>
         </is>
       </c>
       <c r="F148" t="n">
-        <v>17.4949037476</v>
+        <v>0.0009245</v>
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -5642,11 +5642,11 @@
         </is>
       </c>
       <c r="F149" t="n">
-        <v>5.28e-05</v>
+        <v>29.6566178538</v>
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -5677,11 +5677,11 @@
         </is>
       </c>
       <c r="F150" t="n">
-        <v>0.6755396997000001</v>
+        <v>8.76e-05</v>
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -5712,11 +5712,11 @@
         </is>
       </c>
       <c r="F151" t="n">
-        <v>0.8937031935999999</v>
+        <v>1.1140382688</v>
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -5743,15 +5743,15 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>Amazon Simple Storage Service</t>
+          <t>Amazon Simple Queue Service</t>
         </is>
       </c>
       <c r="F152" t="n">
-        <v>17049.7376130621</v>
+        <v>1.4778836006</v>
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -5782,11 +5782,11 @@
         </is>
       </c>
       <c r="F153" t="n">
-        <v>0.0344014105</v>
+        <v>29772.4561384546</v>
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>Environment$Common</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -5817,11 +5817,11 @@
         </is>
       </c>
       <c r="F154" t="n">
-        <v>0.0001237826</v>
+        <v>0.05706919</v>
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>Environment$Dev</t>
+          <t>Environment$Common</t>
         </is>
       </c>
     </row>
@@ -5852,11 +5852,11 @@
         </is>
       </c>
       <c r="F155" t="n">
-        <v>0.084486353</v>
+        <v>0.0002053639</v>
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>Environment$POC</t>
+          <t>Environment$Dev</t>
         </is>
       </c>
     </row>
@@ -5887,11 +5887,11 @@
         </is>
       </c>
       <c r="F156" t="n">
-        <v>0.0176036325</v>
+        <v>0.1117472478</v>
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$POC</t>
         </is>
       </c>
     </row>
@@ -5922,11 +5922,11 @@
         </is>
       </c>
       <c r="F157" t="n">
-        <v>0.0006637898</v>
+        <v>0.0291502625</v>
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>Environment$Sandbox</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -5957,11 +5957,11 @@
         </is>
       </c>
       <c r="F158" t="n">
-        <v>0.0013728063</v>
+        <v>0.0010849642</v>
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>Environment$common</t>
+          <t>Environment$Sandbox</t>
         </is>
       </c>
     </row>
@@ -5992,11 +5992,11 @@
         </is>
       </c>
       <c r="F159" t="n">
-        <v>11.6943588603</v>
+        <v>0.0022535347</v>
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$common</t>
         </is>
       </c>
     </row>
@@ -6027,11 +6027,11 @@
         </is>
       </c>
       <c r="F160" t="n">
-        <v>0.0541490774</v>
+        <v>19.2810082099</v>
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>Environment$loadtest</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -6062,11 +6062,11 @@
         </is>
       </c>
       <c r="F161" t="n">
-        <v>935.7220403403001</v>
+        <v>0.0939962944</v>
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$loadtest</t>
         </is>
       </c>
     </row>
@@ -6097,11 +6097,11 @@
         </is>
       </c>
       <c r="F162" t="n">
-        <v>1.3447410522</v>
+        <v>1533.0006099917</v>
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -6132,11 +6132,11 @@
         </is>
       </c>
       <c r="F163" t="n">
-        <v>9683.9641512911</v>
+        <v>2.2620211094</v>
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -6167,11 +6167,11 @@
         </is>
       </c>
       <c r="F164" t="n">
-        <v>0.000650939</v>
+        <v>15874.672068806</v>
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>Environment$qa</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -6202,11 +6202,11 @@
         </is>
       </c>
       <c r="F165" t="n">
-        <v>0.0016743951</v>
+        <v>0.0010615506</v>
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$qa</t>
         </is>
       </c>
     </row>
@@ -6233,15 +6233,15 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>Amazon Simple Workflow Service</t>
+          <t>Amazon Simple Storage Service</t>
         </is>
       </c>
       <c r="F166" t="n">
-        <v>5.756999999999999e-07</v>
+        <v>0.0027533512</v>
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -6268,11 +6268,11 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>Amazon SimpleDB</t>
+          <t>Amazon Simple Workflow Service</t>
         </is>
       </c>
       <c r="F167" t="n">
-        <v>6.9565e-06</v>
+        <v>9.477e-07</v>
       </c>
       <c r="G167" t="inlineStr">
         <is>
@@ -6303,11 +6303,11 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>Amazon Virtual Private Cloud</t>
+          <t>Amazon SimpleDB</t>
         </is>
       </c>
       <c r="F168" t="n">
-        <v>5473.9708411646</v>
+        <v>1.14445e-05</v>
       </c>
       <c r="G168" t="inlineStr">
         <is>
@@ -6342,11 +6342,11 @@
         </is>
       </c>
       <c r="F169" t="n">
-        <v>0.000256945</v>
+        <v>9201.684943083799</v>
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -6377,11 +6377,11 @@
         </is>
       </c>
       <c r="F170" t="n">
-        <v>89.85264820810001</v>
+        <v>0.000256945</v>
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -6412,11 +6412,11 @@
         </is>
       </c>
       <c r="F171" t="n">
-        <v>1.825</v>
+        <v>148.2161884725</v>
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -6447,11 +6447,11 @@
         </is>
       </c>
       <c r="F172" t="n">
-        <v>95.56999999999999</v>
+        <v>3.01</v>
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -6482,11 +6482,11 @@
         </is>
       </c>
       <c r="F173" t="n">
-        <v>49.8501118865</v>
+        <v>157.55</v>
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>Environment$shared</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -6513,15 +6513,15 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>Amazon WorkSpaces</t>
+          <t>Amazon Virtual Private Cloud</t>
         </is>
       </c>
       <c r="F174" t="n">
-        <v>19</v>
+        <v>82.28246982589999</v>
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$shared</t>
         </is>
       </c>
     </row>
@@ -6548,11 +6548,11 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>AmazonCloudWatch</t>
+          <t>Amazon WorkSpaces</t>
         </is>
       </c>
       <c r="F175" t="n">
-        <v>6563.4848373808</v>
+        <v>19.68</v>
       </c>
       <c r="G175" t="inlineStr">
         <is>
@@ -6587,11 +6587,11 @@
         </is>
       </c>
       <c r="F176" t="n">
-        <v>0.0008980151</v>
+        <v>10808.7931273353</v>
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -6622,11 +6622,11 @@
         </is>
       </c>
       <c r="F177" t="n">
-        <v>455.5424038138</v>
+        <v>0.0008980151</v>
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -6657,11 +6657,11 @@
         </is>
       </c>
       <c r="F178" t="n">
-        <v>2135.9397112853</v>
+        <v>736.7505046688</v>
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -6688,15 +6688,15 @@
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>AmazonWorkMail</t>
+          <t>AmazonCloudWatch</t>
         </is>
       </c>
       <c r="F179" t="n">
-        <v>99.905555474</v>
+        <v>3419.9271846467</v>
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -6723,11 +6723,11 @@
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>CloudWatch Events</t>
+          <t>AmazonWorkMail</t>
         </is>
       </c>
       <c r="F180" t="n">
-        <v>1.3118849355</v>
+        <v>164.69444431</v>
       </c>
       <c r="G180" t="inlineStr">
         <is>
@@ -6758,11 +6758,11 @@
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>Proofpoint Security [Private Offer Only]</t>
+          <t>CloudWatch Events</t>
         </is>
       </c>
       <c r="F181" t="n">
-        <v>49929.72</v>
+        <v>3.2483727296</v>
       </c>
       <c r="G181" t="inlineStr">
         <is>
@@ -6793,11 +6793,11 @@
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>Savings Plans for AWS Compute usage</t>
+          <t>Proofpoint Security [Private Offer Only]</t>
         </is>
       </c>
       <c r="F182" t="n">
-        <v>28800</v>
+        <v>49929.72</v>
       </c>
       <c r="G182" t="inlineStr">
         <is>
@@ -6828,13 +6828,48 @@
       </c>
       <c r="E183" t="inlineStr">
         <is>
+          <t>Savings Plans for AWS Compute usage</t>
+        </is>
+      </c>
+      <c r="F183" t="n">
+        <v>31236</v>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>Environment$</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>JUN</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>Entercom Communications</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>724972922289</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
           <t>Tax</t>
         </is>
       </c>
-      <c r="F183" t="n">
-        <v>7517.26</v>
-      </c>
-      <c r="G183" t="inlineStr">
+      <c r="F184" t="n">
+        <v>10361.77</v>
+      </c>
+      <c r="G184" t="inlineStr">
         <is>
           <t>Environment$</t>
         </is>

</xml_diff>